<commit_message>
Ora cambia pagina fino alla numero 3
</commit_message>
<xml_diff>
--- a/PagineHtml/2-Carta igienica 3 veli 50 m ecologica all'ingrosso | toilet paper 3 ply 50m eco-friendly bulk supplier manufacturer.xlsx
+++ b/PagineHtml/2-Carta igienica 3 veli 50 m ecologica all'ingrosso | toilet paper 3 ply 50m eco-friendly bulk supplier manufacturer.xlsx
@@ -463,66 +463,62 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>All'ingrosso a buon mercato prezzo Papel Higienico ultra morbido vergine pasta di legno 3 strati carta igienica carta da bagno</t>
+          <t>Polpa vergine TPS-V-1000 1 strato 1000 fogli di carta igienica morbida</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0,0693-0,1646 €</t>
+          <t>0,2426 €</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ordine minimo: 20.000 rulli</t>
+          <t>Ordine minimo: 48.000 rulli</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Baoding Zhiruo Hygiene Products Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
+          <t>Shenzhen Anmay Paper Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso carta igienica solubile in acqua morbida e igienica 3 strati bagno tessuto di bambù rotolo di carta igienica</t>
+          <t>3 strati di esportazione bianco vergine carta igienica carta igienica rotolo in magazzino all'ingrosso</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0,1646-0,1906 €</t>
+          <t>0,2166 €</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ordine minimo: 50.000 pacchetti</t>
+          <t>Ordine minimo: 30.000 rulli</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ningbo Riway Imp. &amp; Exp. Co., Ltd.</t>
+          <t>Baoda Paper Enterprise Co., Ltd.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Produttore goffrato sfuso a buon mercato carta igienica su misura Ultra morbida 4 /6/10/12 rotoli carta igienica</t>
+          <t>Commercio all'ingrosso 100% vergine tessuto per l'igiene della polpa ultra morbido 3 strati 4 strati di carta igienica</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0,0434-0,1386 €</t>
+          <t>0,052-0,1646 €</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -544,170 +540,170 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso diretto della fabbrica 1/2/3 strato riciclato/vergine/polpa di bambù goffrato per bagno tessuto molle carta igienica rotolo di carta igienica</t>
+          <t>Commercio all'ingrosso carta igienica solubile in acqua morbida e igienica 3 strati bagno tessuto di bambù rotolo di carta igienica</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0,078-0,1992 €</t>
+          <t>0,1646-0,1906 €</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ordine minimo: 2 rulli</t>
+          <t>Ordine minimo: 50.000 pacchetti</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Shenzhen Telling Commodity Co., Ltd.</t>
+          <t>Ningbo Riway Imp. &amp; Exp. Co., Ltd.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso 3 strati Jumbo bambù carta igienica morbida assorbente ed eco-friendly usa e getta carta velina con imballaggio personalizzato</t>
+          <t>All'ingrosso a buon mercato prezzo Papel Higienico ultra morbido vergine pasta di legno 3 strati carta igienica carta da bagno</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0,4331 €</t>
+          <t>0,0693-0,1646 €</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ordine minimo: 300 parti</t>
+          <t>Ordine minimo: 20.000 rulli</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Henrich (shandong) Health Technology Co., Ltd.</t>
+          <t>Baoding Zhiruo Hygiene Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso della fabbrica eco-friendly di bambù carta igienica usa e getta 1/2/3/4 velina di carta naturale OEM Gsm a buon mercato</t>
+          <t>Commercio all'ingrosso carta igienica 2/3 Ply Tissue Custom pasta di legno prezzo basso produttore di carta igienica</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0,078-0,13 €</t>
+          <t>0,0434-0,1646 €</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ordine minimo: 150.000 rulli</t>
+          <t>Ordine minimo: 20.000 rulli</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fujian Wellcare Hygiene Products Co., Ltd.</t>
+          <t>Baoding Zhiruo Hygiene Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Carta igienica da bagno a 3 strati ecologica personalizzata carta igienica 4 strati all'ingrosso carta toliet</t>
+          <t>Produttori domestici pasta di legno vergine alla rinfusa 3 strati solubile in acqua bagno carta igienica rotolo di carta per ristorante Hotel Office</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0,1213-0,1559 €</t>
+          <t>0,0434-0,1386 €</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ordine minimo: 30.000 rulli</t>
+          <t>Ordine minimo: 2 rulli</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Zhejiang Furuisen Spunlaced Non-Wovens Co., Ltd.</t>
+          <t>Baoding Roushun Trading Co., Ltd.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso 3ply biodegradabile made in China papel higienico riciclato eco tessuto di carta igienica rotolo</t>
+          <t>Produttore goffrato sfuso a buon mercato carta igienica su misura Ultra morbida 4 /6/10/12 rotoli carta igienica</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0,1213 €</t>
+          <t>0,0434-0,1386 €</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1 rullo</t>
+          <t>Ordine minimo: 2 rulli</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Zhucheng Lizhou Paper Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>Baoding Roushun Trading Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ingrosso rotolo di carta igienica di bambù a 3 strati con Logo personalizzato con punto in rilievo con motivo a 2 strati di carta velina per feste</t>
+          <t>Carta igienica biodegradabile per carta igienica portatile In cartapesta da bagno nomi di marca del tessuto acquisto all'ingrosso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0,2166 €</t>
+          <t>0,104 €</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1 rullo</t>
+          <t>Ordine minimo: 48.000 rulli</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Guangzhou Huaching Paper Industrial Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>4.3</t>
-        </is>
-      </c>
+          <t>Shenzhen Anmay Paper Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Morbido organico Eco Friendly certificato OEM personalizzato a buon mercato 4 3 2 strati di carta igienica di bambù rotoli di carta igienica</t>
+          <t>Commercio all'ingrosso diretto della fabbrica 1/2/3 strato riciclato/vergine/polpa di bambù goffrato per bagno tessuto molle carta igienica rotolo di carta igienica</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0,13-0,2166 €</t>
+          <t>0,078-0,1992 €</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -717,51 +713,51 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sichuan Petrochemical Yashi Paper Co., Ltd.</t>
+          <t>Shenzhen Telling Commodity Co., Ltd.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>3.8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carta igienica di bambù Premium 3 strati-rotoli di tessuto da bagno ecologici e morbidi per la casa-all'ingrosso disponibili alla rinfusa</t>
+          <t>Carta igienica biodegradabile a 3 strati di carta igienica con etichetta privata</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0,0347-0,0434 €</t>
+          <t>0,13 €</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ordine minimo: 10 rulli</t>
+          <t>Ordine minimo: 25.000 rulli</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Baoding Yisu Trading Co., Ltd.</t>
+          <t>Chishui Newland Import And Export Trading Co., Ltd.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.7</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3 strati di carta sanitaria inglese imballaggio di pasta di legno vergine di alta qualità eco-friendly commercio all'ingrosso del tessuto rotolo di carta igienica</t>
+          <t>Carta igienica all'ingrosso 2/3 usa e getta carta igienica di pasta di bambù stampata su misura fabbricata a buon mercato carta igienica</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0,026-0,0434 €</t>
+          <t>0,078-0,2166 €</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -771,324 +767,328 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Xi'an Giant Better Hygiene Product Co., Ltd.</t>
+          <t>Baoding Roushun Trading Co., Ltd.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>All'ingrosso Ultra morbido 3 strati del tessuto del bagno FSC ECO Friendly carta igienica della polpa di bambù</t>
+          <t>Commercio all'ingrosso 3 strati Jumbo bambù carta igienica morbida assorbente ed eco-friendly usa e getta carta velina con imballaggio personalizzato</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0,0693-0,1126 €</t>
+          <t>0,4331 €</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ordine minimo: 30.000 rulli</t>
+          <t>Ordine minimo: 300 parti</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Joylife Industry (Dongguan) Co., Ltd.</t>
+          <t>Henrich (shandong) Health Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Rotolo di carta igienica con logo personalizzato</t>
+          <t>Rotolo di tessuto da bagno in rilievo di carta igienica in pasta di legno all'ingrosso biodegradabile a 3 strati</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0,1559-0,2599 €</t>
+          <t>0,0693-0,1992 €</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ordine minimo: 10.000 rulli</t>
+          <t>Ordine minimo: 100 rulli</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Baoding Hozhong Hygienic Products Manufacturing Co., Ltd.</t>
+          <t>Baoding Yusen Sanitary Health Supplies Co., Ltd.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Rotolo di carta igienica 3ply Soft Eco Friendly all'ingrosso</t>
+          <t>Commercio all'ingrosso della fabbrica eco-friendly di bambù carta igienica usa e getta 1/2/3/4 velina di carta naturale OEM Gsm a buon mercato</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0,0044-0,0052 €</t>
+          <t>0,078-0,13 €</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1.000 rulli</t>
+          <t>Ordine minimo: 150.000 rulli</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>H&amp;R BEVERAGES B.V.</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>Fujian Wellcare Hygiene Products Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso a buon mercato prezzo di lusso di qualità carta Tissue 2 3 4 5 strati Eco Friendly per Hotel e uso domestico OEM carta igienica</t>
+          <t>24 rotoli di carta velina commerciale settica sicura 3 strati di carta igienica morbida e forte fatta di polpa di bambù all'ingrosso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0,1126-0,2512 €</t>
+          <t>0,2166 €</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ordine minimo: 10 rulli</t>
+          <t>Ordine minimo: 20.000 parti</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Baoding Wanbang Paper Products Co., Ltd.</t>
+          <t>Qingdao Dongfang Jiarui Int'l Co., Ltd.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.7</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso eco-friendly al 100% pasta di legno vergine 3-strati di carta igienica bagno del tessuto</t>
+          <t>Carta igienica da bagno a 3 strati ecologica personalizzata carta igienica 4 strati all'ingrosso carta toliet</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0,078 €</t>
+          <t>0,1213-0,1559 €</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ordine minimo: 50.000 rulli</t>
+          <t>Ordine minimo: 30.000 rulli</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Lianyungang Jiayun International Trade Co., Ltd.</t>
+          <t>Zhejiang Furuisen Spunlaced Non-Wovens Co., Ltd.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Morbido puro 3 Strati di Rotoli di Carta Igienica Bianco All'ingrosso Affare di Lusso Morbido Sostenibile Del Tessuto</t>
+          <t>Commercio all'ingrosso 3ply biodegradabile made in China papel higienico riciclato eco tessuto di carta igienica rotolo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0,1473-0,2079 €</t>
+          <t>0,1213 €</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ordine minimo: 30.000 rulli</t>
+          <t>Ordine minimo: 1 rullo</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Dongguan Dingqiao Daily Necessities Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+          <t>Zhucheng Lizhou Paper Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fabbrica di bambù pasta di carta igienica eco-friendly Core rotolamento all'ingrosso prezzo basso naturale OEM Gsm 1/2/3/4 velina</t>
+          <t>Ingrosso rotolo di carta igienica di bambù a 3 strati con Logo personalizzato con punto in rilievo con motivo a 2 strati di carta velina per feste</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1,56-2,17 €</t>
+          <t>0,2166 €</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1.000 rulli</t>
+          <t>Ordine minimo: 1 rullo</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PRSVRA LIMITED</t>
+          <t>Guangzhou Huaching Paper Industrial Co., Ltd.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso a buon mercato 3Ply riciclato carta igienica morbida e forte pasta di legno rotolo di carta</t>
+          <t>Morbido organico Eco Friendly certificato OEM personalizzato a buon mercato 4 3 2 strati di carta igienica di bambù rotoli di carta igienica</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0,1213-0,1473 €</t>
+          <t>0,13-0,2166 €</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ordine minimo: 50.000 rulli</t>
+          <t>Ordine minimo: 2 rulli</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Baoding Hozhong Paper Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>Sichuan Petrochemical Yashi Paper Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>All'ingrosso 4 strati forte assorbimento di acqua all'ingrosso alla rinfusa bagno carta igienica</t>
+          <t>Rotolo di tessuto dal fornitore europeo 600 caso carta igienica 500 bobine di fogli In cina cellulosa alta Gsm Jambo Reels sedile a doppio strato</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0,0434-0,1473 €</t>
+          <t>0,1473 €</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ordine minimo: 2 rulli</t>
+          <t>Ordine minimo: 48.000 rulli</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Hebei Kongshi Paper Products Processing Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
+          <t>Shenzhen Anmay Paper Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Carta igienica all'ingrosso,</t>
+          <t>Carta igienica di bambù Premium 3 strati-rotoli di tessuto da bagno ecologici e morbidi per la casa-all'ingrosso disponibili alla rinfusa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0,2599 €</t>
+          <t>0,0347-0,0434 €</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ordine minimo: 100 rulli</t>
+          <t>Ordine minimo: 10 rulli</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Baoding Yusen Sanitary Health Supplies Co., Ltd.</t>
+          <t>Baoding Yisu Trading Co., Ltd.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Polpa vergine TPS-V-1000 1 strato 1000 fogli di carta igienica morbida</t>
+          <t>3 strati di carta sanitaria inglese imballaggio di pasta di legno vergine di alta qualità eco-friendly commercio all'ingrosso del tessuto rotolo di carta igienica</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0,2426 €</t>
+          <t>0,026-0,0434 €</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ordine minimo: 48.000 rulli</t>
+          <t>Ordine minimo: 2 rulli</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Shenzhen Anmay Paper Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>Xi'an Giant Better Hygiene Product Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lampure di bambù carta igienica bassa moq all'ingrosso di alta qualità eco-friendly piena goffratura 3 strati carta igienica vendita alla rinfusa</t>
+          <t>YHC carta igienica all'ingrosso su misura 3ply stampato in pasta di legno rotolo di carta igienica</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0,2599 €</t>
+          <t>0,0867-0,104 €</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ordine minimo: 100 rulli</t>
+          <t>Ordine minimo: 65.000 rulli</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Sichuan Lampure Daily Commodity Co., Ltd.</t>
+          <t>Hebei Yihoucheng Commodity Co., Ltd.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
@@ -1122,12 +1122,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Oem a buon mercato all'ingrosso biodegradabile 1ply 2ply 3ply carta igienica</t>
+          <t>All'ingrosso Ultra morbido 3 strati del tessuto del bagno FSC ECO Friendly carta igienica della polpa di bambù</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0,0607-0,2166 €</t>
+          <t>0,0693-0,1126 €</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Dongguan Jinfong Paper Industry Co., Limited</t>
+          <t>Joylife Industry (Dongguan) Co., Ltd.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1149,126 +1149,130 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso 100% vergine tessuto per l'igiene della polpa ultra morbido 3 strati 4 strati di carta igienica</t>
+          <t>Carta igienica di bambù biologica Logo personalizzato 48 rotolo 3 strati di carta igienica di bambù non sbiancata morbida</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0,052-0,1646 €</t>
+          <t>0,0434-0,1646 €</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ordine minimo: 2 rulli</t>
+          <t>Ordine minimo: 20.000 rulli</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Baoding Roushun Trading Co., Ltd.</t>
+          <t>Baoding Zhiruo Hygiene Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Rotolo di carta igienica a buon mercato all'ingrosso di alta qualità a 3 strati ecologico</t>
+          <t>Rotolo di carta igienica con logo personalizzato</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0,1559-0,2166 €</t>
+          <t>0,1559-0,2599 €</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ordine minimo: 15.000 rulli</t>
+          <t>Ordine minimo: 10.000 rulli</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Quanzhou Blossom Trading Co., Ltd.</t>
+          <t>Baoding Hozhong Hygienic Products Manufacturing Co., Ltd.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso di pulizia su misura 2 strati 3 strati 16 24 pacchetti bagno Tissue rotolo di carta igienica</t>
+          <t>Premio di Qualità Su Misura a buon mercato bagno wc tissue riciclato 3 strati 96 rolls soft touch all'ingrosso pacchetto di carta igienica carta velina</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0,0607-0,1646 €</t>
+          <t>0,1646 €</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ordine minimo: 2 rulli</t>
+          <t>Ordine minimo: 50.000 rulli</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Hebei Kongshi Paper Products Processing Co., Ltd.</t>
+          <t>Dongguan Green Paper Industrial Co., Ltd.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Presa di fabbrica biodegradabile 2ply &amp; 3ply bagno carta igienica fatta con pasta di legno grezzo alla rinfusa</t>
+          <t>Importazione biodegradabile sfusa personalizzata stampata a 3 strati selpak rotolo di carta igienica in tessuto riciclato di bambù economico papel higienico por mayor</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0,1213 €</t>
+          <t>0,0867-0,2685 €</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ordine minimo: 50.000 rulli</t>
+          <t>Ordine minimo: 25.000 rulli</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Xiamen Qiaodou Daily Commodity Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>Shenzhen Telling Commodity Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Carta igienica biodegradabile per carta igienica portatile In cartapesta da bagno nomi di marca del tessuto acquisto all'ingrosso</t>
+          <t>Rotolo di carta igienica 3ply Soft Eco Friendly all'ingrosso</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0,104 €</t>
+          <t>0,0044-0,0052 €</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ordine minimo: 48.000 rulli</t>
+          <t>Ordine minimo: 1.000 rulli</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Shenzhen Anmay Paper Co., Ltd.</t>
+          <t>H&amp;R BEVERAGES B.V.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1276,130 +1280,126 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Logo personalizzato di carta di bambù eco-friendly di alta qualità con 3 strati di tessuto sfuso 2 strati di carta igienica morbida all'ingrosso</t>
+          <t>Commercio all'ingrosso a buon mercato prezzo di lusso di qualità carta Tissue 2 3 4 5 strati Eco Friendly per Hotel e uso domestico OEM carta igienica</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0,0607-0,13 €</t>
+          <t>0,1126-0,2512 €</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ordine minimo: 10.000 parti</t>
+          <t>Ordine minimo: 10 rulli</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Qingdao Dongfang Jiarui Int'l Co., Ltd.</t>
+          <t>Baoding Wanbang Paper Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso carta igienica 2/3 Ply Tissue Custom pasta di legno prezzo basso produttore di carta igienica</t>
+          <t>Commercio all'ingrosso eco-friendly al 100% pasta di legno vergine 3-strati di carta igienica bagno del tessuto</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0,0434-0,1646 €</t>
+          <t>0,078 €</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ordine minimo: 20.000 rulli</t>
+          <t>Ordine minimo: 50.000 rulli</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Baoding Zhiruo Hygiene Products Co., Ltd.</t>
+          <t>Lianyungang Jiayun International Trade Co., Ltd.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Morbido organico 3 strati di carta igienica igienica da bagno tessuto Eco Friendly produttore certificato Oem bagno carta igienica all'ingrosso</t>
+          <t>Commercio all'ingrosso su misura della polpa di bambù 100% usa e getta igienico sanitario rotolo morbido 2ply 3ply 4ply forte goffrato lavabile per</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0,078-0,1733 €</t>
+          <t>0,1473-0,1646 €</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ordine minimo: 5.000 rulli</t>
+          <t>Ordine minimo: 1.000 rulli</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Baoding Yusen Sanitary Health Supplies Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>4.4</t>
-        </is>
-      </c>
+          <t>MEGA TOP INTERNATIONAL LIMITED</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Produttori domestici pasta di legno vergine alla rinfusa 3 strati solubile in acqua bagno carta igienica rotolo di carta per ristorante Hotel Office</t>
+          <t>3ply Whosale carta igienica bianca biologica Eco Friendly certificata all'ingrosso produttore Oem personalizzabile carta igienica da bagno</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0,0434-0,1386 €</t>
+          <t>0,078-0,1819 €</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ordine minimo: 2 rulli</t>
+          <t>Ordine minimo: 5.000 sacchi</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Baoding Roushun Trading Co., Ltd.</t>
+          <t>Baoding Yusen Sanitary Health Supplies Co., Ltd.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Vendita calda 3 strati di bambù non sbiancato rotolo di carta igienica eco-friendly monouso morbido toccante all'ingrosso sfuso</t>
+          <t>Morbido puro 3 Strati di Rotoli di Carta Igienica Bianco All'ingrosso Affare di Lusso Morbido Sostenibile Del Tessuto</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0,1906-0,2166 €</t>
+          <t>0,1473-0,2079 €</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ordine minimo: 10.000 rulli</t>
+          <t>Ordine minimo: 30.000 rulli</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Baoding Yichen Trade Co., Ltd.</t>
+          <t>Dongguan Dingqiao Daily Necessities Co., Ltd.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1411,49 +1411,49 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3 strati di esportazione bianco vergine carta igienica carta igienica rotolo in magazzino all'ingrosso</t>
+          <t>Fabbrica di bambù pasta di carta igienica eco-friendly Core rotolamento all'ingrosso prezzo basso naturale OEM Gsm 1/2/3/4 velina</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0,2166 €</t>
+          <t>1,56-2,17 €</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ordine minimo: 30.000 rulli</t>
+          <t>Ordine minimo: 1.000 rulli</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Baoda Paper Enterprise Co., Ltd.</t>
+          <t>PRSVRA LIMITED</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>100% legno vergine eco-friendly 3 strati 15gsm carta igienica sfusa a buon mercato stampa goffrata 10 rotoli confezionati singolarmente</t>
+          <t>Commercio all'ingrosso a buon mercato 3Ply riciclato carta igienica morbida e forte pasta di legno rotolo di carta</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0,0693-0,2166 €</t>
+          <t>0,1213-0,1473 €</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ordine minimo: 25.000 parti</t>
+          <t>Ordine minimo: 50.000 rulli</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Qingdao Ample Technology Co., Ltd.</t>
+          <t>Baoding Hozhong Paper Co., Ltd.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1461,85 +1461,93 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso di pasta di legno di bambù morbido stampato rotoli Jumbo carta igienica 12/16/24/48 rotoli confezioni 2-3 strati usa e getta FSC</t>
+          <t>Lampure di bambù carta igienica bassa moq all'ingrosso di alta qualità eco-friendly piena goffratura 3 strati carta igienica vendita alla rinfusa</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0,1126-0,2166 €</t>
+          <t>0,2599 €</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ordine minimo: 5.000 rulli</t>
+          <t>Ordine minimo: 100 rulli</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Joylife Industry (Dongguan) Co., Ltd.</t>
+          <t>Sichuan Lampure Daily Commodity Co., Ltd.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.3</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Jumbo Roll fornitore di carta igienica cina vergine pasta di legno alla rinfusa 3 strati Eco tessuto da bagno per alberghi ristoranti</t>
+          <t>Oem a buon mercato all'ingrosso biodegradabile 1ply 2ply 3ply carta igienica</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1,55 €</t>
+          <t>0,0607-0,2166 €</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ordine minimo: 260 chilogrammi</t>
+          <t>Ordine minimo: 30.000 rulli</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Qingdao Shuncai Trading Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>Dongguan Jinfong Paper Industry Co., Limited</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso 3 strati 100g/rotolo pasta di legno vergine carta igienica morbida 10cm fazzoletti lavabili dal produttore</t>
+          <t>Rotolo di carta igienica a buon mercato all'ingrosso di alta qualità a 3 strati ecologico</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0,13 €</t>
+          <t>0,1559-0,2166 €</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ordine minimo: 100 parti</t>
+          <t>Ordine minimo: 15.000 rulli</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Dongguan Xingli Paper Industry Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>Quanzhou Blossom Trading Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Carta igienica all'ingrosso a buon mercato all'ingrosso di alta qualità morbida personalizzata 3 strati all'ingrosso carta igienica eco-friendly</t>
+          <t>Presa di fabbrica biodegradabile 2ply &amp; 3ply bagno carta igienica fatta con pasta di legno grezzo alla rinfusa</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0,1646-0,1733 €</t>
+          <t>0,1213 €</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1549,57 +1557,57 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Quanzhou Yaosheng Paper Products Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
+          <t>Xiamen Qiaodou Daily Commodity Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>La fabbrica personalizza la migliore vendita di carta igienica Jumbo a 3 strati Premium</t>
+          <t>Vendita calda 3 strati di bambù non sbiancato rotolo di carta igienica eco-friendly monouso morbido toccante all'ingrosso sfuso</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0,4851 €</t>
+          <t>0,1906-0,2166 €</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1 rullo</t>
+          <t>Ordine minimo: 10.000 rulli</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Dongguan Xingli Paper Industry Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>Baoding Yichen Trade Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso personalizzato 2ply 3ply goffrato 100% vergine polpa morbida per la pelle-friendly produttore di carta igienica rotolo di carta igienica</t>
+          <t>100% legno vergine eco-friendly 3 strati 15gsm carta igienica sfusa a buon mercato stampa goffrata 10 rotoli confezionati singolarmente</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0,0693-0,3032 €</t>
+          <t>0,0693-0,2166 €</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ordine minimo: 800 rulli</t>
+          <t>Ordine minimo: 25.000 parti</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Dongguan Xingli Paper Industry Co., Ltd.</t>
+          <t>Qingdao Ample Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1607,49 +1615,45 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rotolo di carta igienica personalizzato a 3 strati all'ingrosso ecologico di carta igienica di legno vergine di vendita calda 100%</t>
+          <t>Jumbo Roll fornitore di carta igienica cina vergine pasta di legno alla rinfusa 3 strati Eco tessuto da bagno per alberghi ristoranti</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>13,86-15,99 €</t>
+          <t>1,55 €</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ordine minimo: 100 cartoni</t>
+          <t>Ordine minimo: 260 chilogrammi</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Foshan Bao Shi Jie Hygiene Supplies Co., Ltd.</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+          <t>Qingdao Shuncai Trading Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Commercio all'ingrosso a buon mercato 2ply 3ply rotolo di carta igienica monouso forte lavabile morbido stampato riciclato per bagno sfuso</t>
+          <t>Commercio all'ingrosso personalizzato 2ply 3ply goffrato 100% vergine polpa morbida per la pelle-friendly produttore di carta igienica rotolo di carta igienica</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>0,2512-0,3032 €</t>
+          <t>0,0693-0,3032 €</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ordine minimo: 200.000 sacchi</t>
+          <t>Ordine minimo: 800 rulli</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Guizhou Zhiang Trading Co., Ltd.</t>
+          <t>Dongguan Xingli Paper Industry Co., Ltd.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1657,45 +1661,49 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Rotolo di carta igienica in bambù 100% morbido a 3 strati ecologico certificato e sostenibile</t>
+          <t>Carta igienica all'ingrosso a buon mercato all'ingrosso di alta qualità morbida personalizzata 3 strati all'ingrosso carta igienica eco-friendly</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0,2599-0,3465 €</t>
+          <t>0,1646-0,1733 €</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Ordine minimo: 1.000 rulli</t>
+          <t>Ordine minimo: 50.000 rulli</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>MEGA TOP INTERNATIONAL LIMITED</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>Quanzhou Yaosheng Paper Products Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ingrosso rotolo di carta igienica jumbo bianco riciclato 3 strati di alta qualità</t>
+          <t>Rotolo di carta igienica personalizzato a 3 strati all'ingrosso ecologico di carta igienica di legno vergine di vendita calda 100%</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0,8834 €</t>
+          <t>13,86-15,99 €</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ordine minimo: 14.000 rulli</t>
+          <t>Ordine minimo: 100 cartoni</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Dongguan Green Paper Industrial Co., Ltd.</t>
+          <t>Foshan Bao Shi Jie Hygiene Supplies Co., Ltd.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">

</xml_diff>